<commit_message>
Data Driver First Working Code
</commit_message>
<xml_diff>
--- a/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\FrameworkTemplate\Final-Maven-Framework\TemplatePr2h\src\test\java\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\Final-Maven-Framework-2024\TemplatePr2h2024\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41C267C8-E152-44E6-A050-D66799A98EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5177C1B0-53B2-4525-A51B-A1947A9F2F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -72,39 +72,6 @@
     <t>TC_03</t>
   </si>
   <si>
-    <t>TC_04</t>
-  </si>
-  <si>
-    <t>TC_05</t>
-  </si>
-  <si>
-    <t>TC_06</t>
-  </si>
-  <si>
-    <t>TC_07</t>
-  </si>
-  <si>
-    <t>TC_08</t>
-  </si>
-  <si>
-    <t>TC_09</t>
-  </si>
-  <si>
-    <t>TC_10</t>
-  </si>
-  <si>
-    <t>TC_11</t>
-  </si>
-  <si>
-    <t>TC_12</t>
-  </si>
-  <si>
-    <t>TC_13</t>
-  </si>
-  <si>
-    <t>TC_14</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -112,15 +79,6 @@
   </si>
   <si>
     <t>Homepage</t>
-  </si>
-  <si>
-    <t>Logo</t>
-  </si>
-  <si>
-    <t>Header</t>
-  </si>
-  <si>
-    <t>Contact Us page</t>
   </si>
 </sst>
 </file>
@@ -444,10 +402,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -500,10 +458,10 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -526,7 +484,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -552,298 +510,12 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5" t="s">
-        <v>6</v>
-      </c>
-      <c r="H5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G9" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s">
-        <v>31</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" t="s">
-        <v>31</v>
-      </c>
-      <c r="G11" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" t="s">
-        <v>6</v>
-      </c>
-      <c r="H12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>31</v>
-      </c>
-      <c r="G13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>31</v>
-      </c>
-      <c r="G14" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>25</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H15" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data Driven running on Test Case fix hardcoded
</commit_message>
<xml_diff>
--- a/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\Final-Maven-Framework-2024\TemplatePr2h2024\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5177C1B0-53B2-4525-A51B-A1947A9F2F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40148CC5-9F09-46D5-9E21-C532CC1B133C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -72,13 +72,10 @@
     <t>TC_03</t>
   </si>
   <si>
-    <t>Login</t>
-  </si>
-  <si>
-    <t>Login with incorrect passoword</t>
-  </si>
-  <si>
     <t>Homepage</t>
+  </si>
+  <si>
+    <t>loginTest</t>
   </si>
 </sst>
 </file>
@@ -404,8 +401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +455,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -510,7 +507,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
RowCount issue fixed - Excel Value is taken correctly
</commit_message>
<xml_diff>
--- a/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\Final-Maven-Framework-2024\TemplatePr2h2024\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40148CC5-9F09-46D5-9E21-C532CC1B133C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1887E19-FD81-491A-A191-4B8B1CEB8257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -402,7 +402,7 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -434,6 +434,9 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Number of testcases are taken but not exact "Yes" cases. Taking all the cases
</commit_message>
<xml_diff>
--- a/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\Final-Maven-Framework-2024\TemplatePr2h2024\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1887E19-FD81-491A-A191-4B8B1CEB8257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745CF13C-40E2-4032-993E-BB277A3D51BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -399,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,6 +519,110 @@
         <v>11</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed - Testcases are taken as exact from the excel sheet.
Duplicate calling of the method is removed
</commit_message>
<xml_diff>
--- a/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\Final-Maven-Framework-2024\TemplatePr2h2024\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745CF13C-40E2-4032-993E-BB277A3D51BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871B6637-4E9D-4B39-85FE-8C5E7A6F95F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -72,10 +72,25 @@
     <t>TC_03</t>
   </si>
   <si>
-    <t>Homepage</t>
-  </si>
-  <si>
     <t>loginTest</t>
+  </si>
+  <si>
+    <t>loginTest2</t>
+  </si>
+  <si>
+    <t>Homepage1</t>
+  </si>
+  <si>
+    <t>Homepage2</t>
+  </si>
+  <si>
+    <t>Homepage3</t>
+  </si>
+  <si>
+    <t>Homepage4</t>
+  </si>
+  <si>
+    <t>Homepage5</t>
   </si>
 </sst>
 </file>
@@ -402,7 +417,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -458,7 +473,7 @@
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -510,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
         <v>12</v>
@@ -536,7 +551,7 @@
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
         <v>12</v>
@@ -562,7 +577,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -588,7 +603,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -614,7 +629,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Fixed - only specific testcases should run
Cannot do that with testcases name. Done with group names
</commit_message>
<xml_diff>
--- a/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\Final-Maven-Framework-2024\TemplatePr2h2024\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871B6637-4E9D-4B39-85FE-8C5E7A6F95F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B667E0-697B-4C6D-8943-15F457CF39E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>Homepage2</t>
-  </si>
-  <si>
-    <t>Homepage3</t>
   </si>
   <si>
     <t>Homepage4</t>
@@ -417,7 +414,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,7 +574,7 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
         <v>11</v>
@@ -603,7 +600,7 @@
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
         <v>12</v>
@@ -629,7 +626,7 @@
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G8" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Working Groups- Through excel
</commit_message>
<xml_diff>
--- a/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
+++ b/TemplatePr2h2024/src/test/java/testData/Automation Test Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\prathamesh.lad@nanostuffs.com\Final-Maven-Framework-2024\TemplatePr2h2024\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B667E0-697B-4C6D-8943-15F457CF39E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F23F5B4-39A6-49DF-8D42-59BF7FE7F10F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8916" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="24">
   <si>
     <t>Sr. No.</t>
   </si>
@@ -88,6 +88,15 @@
   </si>
   <si>
     <t>Homepage5</t>
+  </si>
+  <si>
+    <t>Groups</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t>loginTest3</t>
   </si>
 </sst>
 </file>
@@ -414,7 +423,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,7 +456,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="H1" t="s">
         <v>6</v>
@@ -473,7 +482,7 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
         <v>11</v>
@@ -574,10 +583,10 @@
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>

</xml_diff>